<commit_message>
Alterações no doc do tcc - capitulo 1, 2 e 3
</commit_message>
<xml_diff>
--- a/Documentos/Categorização.xlsx
+++ b/Documentos/Categorização.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8010" windowHeight="4575" xr2:uid="{B10FE605-C1B6-4FA0-8C5C-422E37E00AEE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8010" windowHeight="4575" activeTab="1" xr2:uid="{B10FE605-C1B6-4FA0-8C5C-422E37E00AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>10155178125107958_693086137537036</t>
   </si>
@@ -198,13 +200,55 @@
   </si>
   <si>
     <t>13 - Positivo Campanha - Negativo Empresa</t>
+  </si>
+  <si>
+    <t>Positivo Campanha - Empresa</t>
+  </si>
+  <si>
+    <t>Positivo Campanha - Negativo Empresa</t>
+  </si>
+  <si>
+    <t>Negativo Campanha - Empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t>Outras marcas - negativo</t>
+  </si>
+  <si>
+    <t>Outras marcas - positivo</t>
+  </si>
+  <si>
+    <t>Socialização entre usuários</t>
+  </si>
+  <si>
+    <t>Socialização/Pedidos/Sugestões - Skol</t>
+  </si>
+  <si>
+    <t>Positivo Empresa - Skol</t>
+  </si>
+  <si>
+    <t>Positivo Campanha - Reposter</t>
+  </si>
+  <si>
+    <t>Negativo Campanha - Reposter</t>
+  </si>
+  <si>
+    <t>Negativo Empresa - Skol</t>
+  </si>
+  <si>
+    <t>Assuntos Diversos / Neutros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +277,31 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +314,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -297,11 +370,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -328,14 +482,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF66FF"/>
       <color rgb="FFFF2D2D"/>
       <color rgb="FFFF5B5B"/>
       <color rgb="FFCCFF99"/>
@@ -376,8 +585,56 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$C$26" max="30000" page="10" val="43"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$5" max="30000" page="10" val="201"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$7" max="30000" page="10" val="9"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$6" max="30000" page="10" val="47"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$9" max="30000" page="10" val="8"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$11" max="30000" page="10" val="21"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$10" max="30000" page="10" val="15"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$C$4" max="30000" page="10" val="10"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$13" max="30000" page="10" val="8"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$15" max="30000" page="10" val="53"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$17" max="30000" page="10" val="8"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$19" max="30000" page="10" val="5"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$21" max="30000" page="10" val="82"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$K$8" max="30000" page="10" val="43"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,13 +674,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>1190625</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>409576</xdr:rowOff>
+          <xdr:rowOff>409575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -433,7 +690,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798D1165-BAA3-4D04-9E23-16986783D536}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -483,7 +740,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC08DC10-810C-4CDF-B57F-08463D7DA65A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -533,7 +790,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B01595DE-D1EA-48BE-8198-C4F9F0A4F16C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -583,7 +840,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{793DAE48-36D2-4456-9EBD-ACAB7197C045}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -633,7 +890,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C73D331-08E9-4BA0-95A6-3CF46F35A34B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -683,7 +940,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5536C86-B27B-4CB6-B386-A8CD4D932622}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -733,7 +990,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{899E7F25-A29F-4D92-9898-1B176CC2DC55}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -767,13 +1024,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>1190625</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>409576</xdr:rowOff>
+          <xdr:rowOff>409575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -783,7 +1040,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42916F1B-4411-4836-B8B2-E31676053DD4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -833,7 +1090,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD46B25C-49B5-4E37-B471-C20F08F10A98}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -883,7 +1140,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156563BC-A23D-41EA-A002-274E4A5A7C0F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -933,7 +1190,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7478C8BE-B9EA-4940-958E-C5449168A0F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -983,7 +1240,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{984E00DF-B762-4DC4-AAEC-688F3DB18623}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1033,7 +1290,612 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0DDEA46-6B0F-463B-A695-33019DCE8AFF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>5196</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>247403</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>222045</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Spinner 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6877C132-717C-49A4-84B2-1B77AC8A477C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>4330</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>247403</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>220188</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Spinner 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDC8B415-3AF1-432B-981B-517087BEA390}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>238989</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Spinner 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4644ECC-8C62-4F6B-A762-483112F92E9D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>4330</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>248515</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Spinner 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E383621-5592-4349-B238-F4FCB9F23DF9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>248515</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2053" name="Spinner 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2031B1F8-42A6-4F7A-8EDF-8F76A084A35D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>4330</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>238990</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Spinner 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9707F739-5D85-48E4-83EC-A196923275DF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>8659</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>246784</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2055" name="Spinner 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8708CC8-F3D0-4F88-AB0D-66869B497D02}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>252845</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>224270</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2056" name="Spinner 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2056"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D12804-6F05-4A24-9DEF-34EBAA1EED38}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>4328</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>248515</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2057" name="Spinner 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A855205D-D56C-484E-9EAC-B3A6D3AC2409}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>248515</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Spinner 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B540BC-85E3-4E37-B328-166A1CB4CCCE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>248515</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2059" name="Spinner 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C99FD00-7072-414C-BB91-69459B61050F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>4329</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>4329</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>238990</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>219940</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2061" name="Spinner 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328D1553-8748-4B21-B5DC-92EBFBC14D34}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1363,8 +2225,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F28" sqref="A1:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1977,4 +2839,648 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF0CAF1-F9E5-416D-AF61-B02214930671}">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="12" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="1.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="1.5703125" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="1.42578125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="1.140625" style="12" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+    </row>
+    <row r="4" spans="1:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="40"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="34"/>
+    </row>
+    <row r="5" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="18">
+        <v>201</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="34"/>
+    </row>
+    <row r="6" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="J6" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="18">
+        <v>47</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="34"/>
+    </row>
+    <row r="7" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>2</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="18">
+        <v>9</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>13</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="J8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="18">
+        <v>43</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="34"/>
+    </row>
+    <row r="9" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>4</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="18">
+        <v>8</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="34"/>
+    </row>
+    <row r="10" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>6</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="J10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="18">
+        <v>15</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="34"/>
+    </row>
+    <row r="11" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="18">
+        <v>21</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="34"/>
+    </row>
+    <row r="12" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="40"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="34"/>
+    </row>
+    <row r="13" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>7</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="18">
+        <v>8</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="J13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="42">
+        <f>SUM(K6:K10,F5:F21)</f>
+        <v>500</v>
+      </c>
+      <c r="M13" s="25"/>
+      <c r="N13" s="34"/>
+    </row>
+    <row r="14" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="40"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="34"/>
+    </row>
+    <row r="15" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>8</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="18">
+        <v>53</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="34"/>
+    </row>
+    <row r="16" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="40"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="34"/>
+    </row>
+    <row r="17" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>9</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="18">
+        <v>8</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="34"/>
+    </row>
+    <row r="18" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="40"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="13"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="34"/>
+    </row>
+    <row r="19" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>10</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="18">
+        <v>5</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="34"/>
+    </row>
+    <row r="20" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="40"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="13"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="34"/>
+    </row>
+    <row r="21" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>43080</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="18">
+        <v>82</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="34"/>
+    </row>
+    <row r="22" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="40"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="34"/>
+    </row>
+    <row r="23" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="12"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="12"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="12"/>
+      <c r="F27" s="13">
+        <f>SUM(F4:F23)</f>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId4" name="Spinner 1">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2050" r:id="rId5" name="Spinner 2">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId6" name="Spinner 3">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2052" r:id="rId7" name="Spinner 4">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2053" r:id="rId8" name="Spinner 5">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId9" name="Spinner 6">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2055" r:id="rId10" name="Spinner 7">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2056" r:id="rId11" name="Spinner 18">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>228600</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2057" r:id="rId12" name="Spinner 19">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2058" r:id="rId13" name="Spinner 20">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2059" r:id="rId14" name="Spinner 24">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2061" r:id="rId15" name="Spinner 26">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>219075</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>